<commit_message>
Mi logt y task para semana 2 de ciclo 2
</commit_message>
<xml_diff>
--- a/tspi/ciclo-2/logt2/20105914.xlsx
+++ b/tspi/ciclo-2/logt2/20105914.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="400"/>
   </bookViews>
   <sheets>
     <sheet name="LOGT1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Curso basico de Ruby</t>
+  </si>
+  <si>
+    <t>23/10/2014</t>
+  </si>
+  <si>
+    <t>Physical Data Model</t>
+  </si>
+  <si>
+    <t>25/10/2015</t>
+  </si>
+  <si>
+    <t>Cycle Report</t>
   </si>
 </sst>
 </file>
@@ -164,18 +176,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -202,6 +202,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,122 +546,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK7"/>
+  <dimension ref="A1:AMK9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="3" width="10.83203125" style="6"/>
-    <col min="4" max="5" width="10.83203125" style="7"/>
-    <col min="6" max="7" width="10.83203125" style="8"/>
-    <col min="8" max="8" width="10.83203125" style="9"/>
-    <col min="9" max="1025" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="3"/>
+    <col min="6" max="7" width="10.83203125" style="4"/>
+    <col min="8" max="8" width="10.83203125" style="5"/>
+    <col min="9" max="1025" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="14"/>
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="15">
         <v>41923</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:8" ht="13">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="16"/>
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="17"/>
     </row>
-    <row r="3" spans="1:8" ht="13">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="E3" s="11" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="17">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="17"/>
     </row>
-    <row r="5" spans="1:8" ht="13">
-      <c r="E5" s="7">
+    <row r="5" spans="1:8">
+      <c r="E5" s="3">
         <f>SUM(E7:E9)/60</f>
-        <v>1.25</v>
+        <v>3.75</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="26">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="2">
         <v>0.75</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="2">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="3">
         <v>30</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <f>((HOUR(C7)-HOUR(B7))*60)+(MINUTE(C7)-MINUTE(B7))-D7</f>
         <v>75</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <v>41</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="5" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="26">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D8" s="3">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3">
+        <f>((HOUR(C8)-HOUR(B8))*60)+(MINUTE(C8)-MINUTE(B8))-D8</f>
+        <v>110</v>
+      </c>
+      <c r="F8" s="4">
+        <v>37</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="26">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <f>((HOUR(C9)-HOUR(B9))*60)+(MINUTE(C9)-MINUTE(B9))-D9</f>
+        <v>40</v>
+      </c>
+      <c r="F9" s="4">
+        <v>45</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>